<commit_message>
add BOM and pi installation directions files
</commit_message>
<xml_diff>
--- a/docs/static/BillOfMaterials.xlsx
+++ b/docs/static/BillOfMaterials.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Dome Slit Mechanism" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,7 +14,8 @@
     <sheet name="Web Cams" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Dome controllers" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Mounting boxes" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Total Costs" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Optional POE" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Total Costs" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="97">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -160,10 +161,10 @@
     <t xml:space="preserve">Subtotal</t>
   </si>
   <si>
-    <t xml:space="preserve">Your choice of weather station; remember to get one compatible with </t>
+    <t xml:space="preserve">Your choice of weather station; remember to get one compatible with WeeWX and that has interior temperature and humidity </t>
   </si>
   <si>
-    <t xml:space="preserve"> WeeWX and that has interior temperature and humidity</t>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">Ambient Weather WS-1400-IP Observer</t>
@@ -214,6 +215,9 @@
     <t xml:space="preserve">SPDT switch</t>
   </si>
   <si>
+    <t xml:space="preserve">Encoder for dome</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dome slit controller mounting box</t>
   </si>
   <si>
@@ -244,6 +248,54 @@
     <t xml:space="preserve">Mounting hardware</t>
   </si>
   <si>
+    <t xml:space="preserve">Ubiquiti EdgeRouter X x ER-X-SFP-US (6 ports)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macroreer for Ubiquiti Gigabit RJ45 Copper SFP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you want copper backhaul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SFP cable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whatever you need for backhaul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ubiquiti Networks 8-Port UniFi Switch, Managed PoE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alternate for more ports</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POE &amp; SFP may be wise to simplify cabling and protect against lightning destroying more than necessary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ports:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raspberry Pi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weather station</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Main camera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guide camera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Back haul</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dome Slit Mechanism</t>
   </si>
   <si>
@@ -260,6 +312,9 @@
   </si>
   <si>
     <t xml:space="preserve">Mounting boxes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optional POE</t>
   </si>
   <si>
     <t xml:space="preserve">Total</t>
@@ -405,7 +460,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -526,6 +581,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -545,7 +604,7 @@
   </sheetPr>
   <dimension ref="1:15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -8975,7 +9034,7 @@
   <dimension ref="1:12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -9031,11 +9090,11 @@
         <v>9.95</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="19" t="n">
         <f aca="false">B4*C4</f>
-        <v>9.95</v>
+        <v>0</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>33</v>
@@ -9064,14 +9123,16 @@
         <v>36</v>
       </c>
       <c r="B6" s="19" t="n">
+        <f aca="false">'Optional POE'!B4</f>
         <v>40.62</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>1</v>
+        <f aca="false">'Optional POE'!C4</f>
+        <v>0</v>
       </c>
       <c r="D6" s="19" t="n">
         <f aca="false">B6*C6</f>
-        <v>40.62</v>
+        <v>0</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>37</v>
@@ -9134,7 +9195,7 @@
       </c>
       <c r="D12" s="23" t="n">
         <f aca="false">SUM(D3:D11)</f>
-        <v>125.27</v>
+        <v>74.7</v>
       </c>
     </row>
   </sheetData>
@@ -9162,7 +9223,7 @@
   <dimension ref="1:10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -9439,10 +9500,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:9"/>
+  <dimension ref="1:10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -9551,14 +9612,39 @@
       <c r="A7" s="0" t="s">
         <v>61</v>
       </c>
+      <c r="B7" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="23" t="n">
+        <f aca="false">B7*C7</f>
+        <v>2</v>
+      </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="22" t="s">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="23" t="n">
+        <v>29</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="23" t="n">
+        <f aca="false">B8*C8</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="23" t="n">
+      <c r="D10" s="23" t="n">
         <f aca="false">SUM(D2:D7)</f>
-        <v>298.28</v>
+        <v>300.28</v>
       </c>
     </row>
   </sheetData>
@@ -9586,7 +9672,7 @@
   <dimension ref="1:13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -9616,7 +9702,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B3" s="23" t="n">
         <v>50</v>
@@ -9631,7 +9717,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B4" s="23" t="n">
         <v>20</v>
@@ -9646,7 +9732,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B5" s="23" t="n">
         <v>100</v>
@@ -9664,7 +9750,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B6" s="23" t="n">
         <v>20</v>
@@ -9677,12 +9763,12 @@
         <v>20</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B7" s="23" t="n">
         <v>35</v>
@@ -9695,12 +9781,12 @@
         <v>35</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C8" s="29" t="n">
         <v>0</v>
@@ -9710,12 +9796,12 @@
         <v>0</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B9" s="23" t="n">
         <v>5</v>
@@ -9753,10 +9839,203 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="1:18"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.1785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="13.3367346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AMJ1" s="21"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="23" t="n">
+        <v>72.99</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="23" t="n">
+        <f aca="false">B3*C3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="19" t="n">
+        <v>40.62</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="19" t="n">
+        <f aca="false">B4*C4</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="23" t="n">
+        <v>19.99</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="23" t="n">
+        <f aca="false">B5*C5</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="23" t="n">
+        <f aca="false">B6*C6</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="23" t="n">
+        <v>184.99</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="23" t="n">
+        <f aca="false">B7*C7</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="23" t="n">
+        <f aca="false">D3+D5+D6+D7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="23" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="23" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="23" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" display="Ubiquiti EdgeRouter X x ER-X-SFP-US (6 ports)"/>
+    <hyperlink ref="A4" r:id="rId2" display="PI PoE Switch HAT – Power over Ethernet"/>
+    <hyperlink ref="A5" r:id="rId3" display="Macroreer for Ubiquiti Gigabit RJ45 Copper SFP"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="1:12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -9788,7 +10067,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="B3" s="23" t="n">
         <f aca="false">'Dome Slit Mechanism'!E15</f>
@@ -9804,23 +10083,23 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="B4" s="23" t="n">
         <f aca="false">'Weather Controller'!D12</f>
-        <v>125.27</v>
+        <v>74.7</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D4" s="23" t="n">
         <f aca="false">B4*C4</f>
-        <v>125.27</v>
+        <v>74.7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="B5" s="23" t="n">
         <f aca="false">'Weather Station'!D10</f>
@@ -9836,7 +10115,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="B6" s="23" t="n">
         <f aca="false">'Web Cams'!D8</f>
@@ -9852,23 +10131,23 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="B7" s="23" t="n">
-        <f aca="false">'Dome controllers'!D9</f>
-        <v>298.28</v>
+        <f aca="false">'Dome controllers'!D10</f>
+        <v>300.28</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D7" s="23" t="n">
         <f aca="false">B7*C7</f>
-        <v>298.28</v>
+        <v>300.28</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="B8" s="23" t="n">
         <f aca="false">'Mounting boxes'!D13</f>
@@ -9882,13 +10161,22 @@
         <v>230</v>
       </c>
     </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="23" t="n">
+        <f aca="false">'Optional POE'!D9</f>
+        <v>0</v>
+      </c>
+    </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="D12" s="23" t="n">
         <f aca="false">SUM(D3:D11)</f>
-        <v>1377.04</v>
+        <v>1328.47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>